<commit_message>
Test Report Result Table
</commit_message>
<xml_diff>
--- a/OpenSource OrangeHRM Test Case Report.xlsx
+++ b/OpenSource OrangeHRM Test Case Report.xlsx
@@ -1,23 +1,98 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>OrangeHRM</t>
+  </si>
+  <si>
+    <t>Module Name</t>
+  </si>
+  <si>
+    <t>Sign In</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Developer Name(TL)</t>
+  </si>
+  <si>
+    <t>Test Executed By</t>
+  </si>
+  <si>
+    <t>TC Start Date</t>
+  </si>
+  <si>
+    <t>TC End Date</t>
+  </si>
+  <si>
+    <t>Test Case Developed By</t>
+  </si>
+  <si>
+    <t>Test Case Reviewed By</t>
+  </si>
+  <si>
+    <t>Muhammed Nayeem</t>
+  </si>
+  <si>
+    <t>TC Execution Start Date</t>
+  </si>
+  <si>
+    <t>TC Execution End Date</t>
+  </si>
+  <si>
+    <t>Browser(Tested)</t>
+  </si>
+  <si>
+    <t>Performance(Tested)</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
+  </si>
+  <si>
+    <t>Out Of Scope</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +100,95 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -42,60 +196,193 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Angles">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="434342"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="CDD7D9"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="797B7E"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="F96A1B"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="08A1D9"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="7C984A"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="C2AD8D"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="506E94"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="5F5F5F"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="969696"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -343,37 +630,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="10">
+        <v>45319</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="10">
+        <v>45320</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="10">
+        <v>45319</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="10">
+        <v>45320</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Project OrangeHRM Test Case Report Done
</commit_message>
<xml_diff>
--- a/OpenSource OrangeHRM Test Case Report.xlsx
+++ b/OpenSource OrangeHRM Test Case Report.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Qjv2CSBdyFojnVocT9h5/dLtA8Z6M1694cxx1fE+KB4="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FWZmraRSjZbr8pIGOyo5pHr2BAr3OSQNZNpEtPQDhPs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="64">
   <si>
     <t>Product Name</t>
   </si>
@@ -30,13 +30,13 @@
     <t>TC Execution Start Date</t>
   </si>
   <si>
-    <t>Test Cases</t>
+    <t>Test Case</t>
   </si>
   <si>
     <t>Module Name</t>
   </si>
   <si>
-    <t>Sign In</t>
+    <t>Login</t>
   </si>
   <si>
     <t>TC End Date</t>
@@ -45,7 +45,7 @@
     <t>TC Execution End Date</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>Pass</t>
   </si>
   <si>
     <t>Epic</t>
@@ -63,7 +63,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>Fail</t>
   </si>
   <si>
     <t>Developer Name(TL)</t>
@@ -87,13 +87,13 @@
     <t>Out Of Scope</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>Total Cases</t>
   </si>
   <si>
     <t>Test Case Id</t>
   </si>
   <si>
-    <t>Modules</t>
+    <t>Module</t>
   </si>
   <si>
     <t>Type Of Testing</t>
@@ -105,7 +105,7 @@
     <t>Test Case Description</t>
   </si>
   <si>
-    <t>Test Scenario</t>
+    <t>Test Case Scenario</t>
   </si>
   <si>
     <t>Expected Result</t>
@@ -132,17 +132,133 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Pass</t>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t>Functional Testing</t>
+  </si>
+  <si>
+    <t>To check login system functionality of OrangeHRM website</t>
+  </si>
+  <si>
+    <t>Valid Username and Valid Password</t>
+  </si>
+  <si>
+    <t>Should be login</t>
+  </si>
+  <si>
+    <t>Found as per expectation</t>
+  </si>
+  <si>
+    <t>Admin
+admin123</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">. Go to this url:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+        <u/>
+      </rPr>
+      <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
+    </r>
+  </si>
+  <si>
+    <t>Invalid Username and Valid Password</t>
+  </si>
+  <si>
+    <t>Should not be login</t>
+  </si>
+  <si>
+    <t>Admin@home
+admin123</t>
+  </si>
+  <si>
+    <t>Valid Username and Invalid Password</t>
+  </si>
+  <si>
+    <t>Admin
+admin12345</t>
+  </si>
+  <si>
+    <t>Invalid Username and Invalid Password</t>
+  </si>
+  <si>
+    <t>Admin_home
+admin12345</t>
+  </si>
+  <si>
+    <t>Blank Username and Password</t>
+  </si>
+  <si>
+    <t>Should not be allow login and display an error warning</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Login Button clickable or not</t>
+  </si>
+  <si>
+    <t>Should be clickable</t>
+  </si>
+  <si>
+    <t>Forgot password link work or not</t>
+  </si>
+  <si>
+    <t>Should be work and navigate to reset password page</t>
+  </si>
+  <si>
+    <t>1. Go to this url:
+https://opensource-demo.orangehrmlive.com/web/index.php/auth/requestPasswordResetCode</t>
+  </si>
+  <si>
+    <t>Checking pasword is masked or not</t>
+  </si>
+  <si>
+    <t>Should be masked when type password</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t xml:space="preserve">1. Go to this url:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <sz val="12.0"/>
+        <u/>
+      </rPr>
+      <t>https://opensource-demo.orangehrmlive.com/web/index.php/auth/login</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -167,15 +283,11 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -188,15 +300,31 @@
       <name val="Cambria"/>
     </font>
     <font>
+      <sz val="12.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12.0"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="11">
@@ -244,14 +372,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor theme="7"/>
+        <fgColor rgb="FFF96A1B"/>
+        <bgColor rgb="FFF96A1B"/>
       </patternFill>
     </fill>
     <fill>
@@ -260,8 +382,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF134F5C"/>
+        <bgColor rgb="FF134F5C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border/>
     <border>
       <left style="thin">
@@ -292,65 +420,108 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -363,54 +534,108 @@
     <xf borderId="1" fillId="3" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="3" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="3" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="8" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,16 +907,8 @@
     <col customWidth="1" min="3" max="3" width="26.14"/>
     <col customWidth="1" min="4" max="4" width="24.86"/>
     <col customWidth="1" min="5" max="5" width="26.71"/>
-    <col customWidth="1" min="6" max="6" width="23.0"/>
-    <col customWidth="1" min="7" max="7" width="17.71"/>
-    <col customWidth="1" min="8" max="8" width="36.71"/>
-    <col customWidth="1" min="9" max="9" width="26.14"/>
-    <col customWidth="1" min="10" max="10" width="35.43"/>
-    <col customWidth="1" min="11" max="11" width="22.14"/>
-    <col customWidth="1" min="12" max="12" width="25.86"/>
-    <col customWidth="1" min="13" max="13" width="20.57"/>
-    <col customWidth="1" min="14" max="14" width="79.71"/>
-    <col customWidth="1" min="15" max="26" width="8.71"/>
+    <col customWidth="1" min="6" max="6" width="35.14"/>
+    <col customWidth="1" min="7" max="40" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="29.25" customHeight="1">
@@ -710,19 +927,22 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="4">
         <v>45320.0</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" ht="30.0" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -734,143 +954,616 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="9">
         <v>45320.0</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" ht="29.25" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
     </row>
     <row r="4" ht="29.25" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="15"/>
       <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" ht="30.0" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="8"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="11">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
     </row>
     <row r="6" ht="29.25" customHeight="1">
-      <c r="G6" s="19" t="s">
+      <c r="F6" s="20"/>
+      <c r="G6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="11">
+        <v>8.0</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" ht="31.5" customHeight="1">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="X7" s="7"/>
+      <c r="Y7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="20" t="s">
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="21"/>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="7"/>
     </row>
-    <row r="8" ht="44.25" customHeight="1">
-      <c r="M8" s="22" t="s">
+    <row r="8" ht="100.5" customHeight="1">
+      <c r="A8" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>38</v>
       </c>
+      <c r="C8" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z8" s="33"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="34"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="34"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="34"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="7"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="9" ht="87.75" customHeight="1">
+      <c r="A9" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="37"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="34"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="34"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="7"/>
+    </row>
+    <row r="10" ht="87.0" customHeight="1">
+      <c r="A10" s="39">
+        <v>3.0</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="37"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="34"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="34"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="6"/>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="7"/>
+    </row>
+    <row r="11" ht="87.75" customHeight="1">
+      <c r="A11" s="39">
+        <v>4.0</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="37"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="34"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="34"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="34"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="6"/>
+      <c r="AL11" s="6"/>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="7"/>
+    </row>
+    <row r="12" ht="89.25" customHeight="1">
+      <c r="A12" s="25">
+        <v>5.0</v>
+      </c>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="37"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="34"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="34"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="34"/>
+      <c r="AJ12" s="6"/>
+      <c r="AK12" s="6"/>
+      <c r="AL12" s="6"/>
+      <c r="AM12" s="6"/>
+      <c r="AN12" s="7"/>
+    </row>
+    <row r="13" ht="90.75" customHeight="1">
+      <c r="A13" s="25">
+        <v>6.0</v>
+      </c>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="42"/>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="34"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="34"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="34"/>
+      <c r="AJ13" s="6"/>
+      <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
+      <c r="AM13" s="6"/>
+      <c r="AN13" s="7"/>
+    </row>
+    <row r="14" ht="84.0" customHeight="1">
+      <c r="A14" s="25">
+        <v>7.0</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="34"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="34"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="34"/>
+      <c r="AJ14" s="6"/>
+      <c r="AK14" s="6"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="7"/>
+    </row>
+    <row r="15" ht="105.0" customHeight="1">
+      <c r="A15" s="25">
+        <v>8.0</v>
+      </c>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="34"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="34"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="34"/>
+      <c r="AJ15" s="6"/>
+      <c r="AK15" s="6"/>
+      <c r="AL15" s="6"/>
+      <c r="AM15" s="6"/>
+      <c r="AN15" s="7"/>
+    </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -1848,37 +2541,157 @@
     <row r="990" ht="15.75" customHeight="1"/>
     <row r="991" ht="15.75" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="M8">
+  <mergeCells count="96">
+    <mergeCell ref="AF14:AH14"/>
+    <mergeCell ref="AF15:AH15"/>
+    <mergeCell ref="AF16:AH16"/>
+    <mergeCell ref="AF17:AH17"/>
+    <mergeCell ref="AF18:AH18"/>
+    <mergeCell ref="AF7:AH7"/>
+    <mergeCell ref="AF8:AH8"/>
+    <mergeCell ref="AF9:AH9"/>
+    <mergeCell ref="AF10:AH10"/>
+    <mergeCell ref="AF11:AH11"/>
+    <mergeCell ref="AF12:AH12"/>
+    <mergeCell ref="AF13:AH13"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="E8:F15"/>
+    <mergeCell ref="D8:D15"/>
+    <mergeCell ref="C8:C15"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="G12:L12"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="G14:L14"/>
+    <mergeCell ref="G15:L15"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="M9:Q9"/>
+    <mergeCell ref="M10:Q10"/>
+    <mergeCell ref="M11:Q11"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="R14:V14"/>
+    <mergeCell ref="R15:V15"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="R8:V8"/>
+    <mergeCell ref="R9:V9"/>
+    <mergeCell ref="R10:V10"/>
+    <mergeCell ref="R11:V11"/>
+    <mergeCell ref="R12:V12"/>
+    <mergeCell ref="R13:V13"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="Y14:AA14"/>
+    <mergeCell ref="Y15:AA15"/>
+    <mergeCell ref="Y7:AA7"/>
+    <mergeCell ref="Y8:AA13"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AB15:AC15"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AB10:AC10"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB13:AC13"/>
+    <mergeCell ref="AD14:AE14"/>
+    <mergeCell ref="AD15:AE15"/>
+    <mergeCell ref="AD7:AE7"/>
+    <mergeCell ref="AD8:AE8"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AD10:AE10"/>
+    <mergeCell ref="AD11:AE11"/>
+    <mergeCell ref="AD12:AE12"/>
+    <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="AI14:AN14"/>
+    <mergeCell ref="AI15:AN15"/>
+    <mergeCell ref="AI7:AN7"/>
+    <mergeCell ref="AI8:AN8"/>
+    <mergeCell ref="AI9:AN9"/>
+    <mergeCell ref="AI10:AN10"/>
+    <mergeCell ref="AI11:AN11"/>
+    <mergeCell ref="AI12:AN12"/>
+    <mergeCell ref="AI13:AN13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="AF8:AH8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
+  <conditionalFormatting sqref="AF8:AH8">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
+  <conditionalFormatting sqref="AF8:AH8">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Not Executed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8">
+  <conditionalFormatting sqref="AF8:AH8">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Out Of Scope"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AF9:AH15">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF9:AH15">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF9:AH15">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+      <formula>"Not Executed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF9:AH15">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>"Out Of Scope"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="AF8:AF15">
       <formula1>"Pass,Fail,Not Executed,Out Of Scope"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>
+    <hyperlink r:id="rId2" ref="Y8"/>
+    <hyperlink r:id="rId3" ref="Y15"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>